<commit_message>
added training and testing performance
</commit_message>
<xml_diff>
--- a/HW_6/results/Summary.xlsx
+++ b/HW_6/results/Summary.xlsx
@@ -230,34 +230,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.64"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="C3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="0" t="s">
         <v>3</v>
       </c>
     </row>
@@ -265,7 +265,10 @@
       <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="B4" s="0" t="n">
+        <v>0.3008</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>0.3227</v>
       </c>
     </row>
@@ -273,7 +276,10 @@
       <c r="A5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="B5" s="0" t="n">
+        <v>0.0763</v>
+      </c>
+      <c r="C5" s="0" t="n">
         <v>0.1503</v>
       </c>
     </row>
@@ -281,7 +287,10 @@
       <c r="A6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="B6" s="0" t="n">
+        <v>0.2038</v>
+      </c>
+      <c r="C6" s="0" t="n">
         <v>0.2102</v>
       </c>
     </row>
@@ -289,7 +298,10 @@
       <c r="A7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="B7" s="0" t="n">
+        <v>0.3223</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <v>0.2754</v>
       </c>
     </row>
@@ -297,7 +309,10 @@
       <c r="A8" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="B8" s="0" t="n">
+        <v>0.4291</v>
+      </c>
+      <c r="C8" s="0" t="n">
         <v>0.2191</v>
       </c>
     </row>
@@ -305,7 +320,10 @@
       <c r="A9" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="B9" s="0" t="n">
+        <v>0.6494</v>
+      </c>
+      <c r="C9" s="0" t="n">
         <v>0.1677</v>
       </c>
     </row>
@@ -313,7 +331,10 @@
       <c r="A10" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="B10" s="0" t="n">
+        <v>0.9347</v>
+      </c>
+      <c r="C10" s="0" t="n">
         <v>0.1624</v>
       </c>
     </row>
@@ -321,7 +342,10 @@
       <c r="A11" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="B11" s="0" t="n">
+        <v>0.9357</v>
+      </c>
+      <c r="C11" s="0" t="n">
         <v>0.1653</v>
       </c>
     </row>
@@ -329,13 +353,16 @@
       <c r="A12" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="B12" s="0" t="n">
+        <v>0.3852</v>
+      </c>
+      <c r="C12" s="0" t="n">
         <v>0.3117</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>